<commit_message>
Code Improved and resource updated
1. Added rarity distinction for operators
2. Uploaded rarity related resources
</commit_message>
<xml_diff>
--- a/Source/arkD.xlsx
+++ b/Source/arkD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37b141e1e60375e0/Arknights/ArknightsIDcard-Ebranch/ArknightsIDCard/Source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{D861895D-AD59-4EF0-B080-FE50D6EF8705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{814B3C94-39B1-4CF3-83FF-05EFABBEC644}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{D861895D-AD59-4EF0-B080-FE50D6EF8705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D789370-B3A5-401E-9586-DBD58A2836DB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,34 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="190">
   <si>
-    <t>等级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>精英化</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>星级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技能一等级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技能二等级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技能三等级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>潜能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>陈</t>
   </si>
   <si>
@@ -193,10 +165,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>模组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>名称：</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -233,10 +201,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>示例：</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -264,10 +228,6 @@
     <t>归溟幽灵鲨</t>
   </si>
   <si>
-    <t>皮肤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>选菜单</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -295,10 +255,6 @@
   </si>
   <si>
     <t>间隙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>模组等级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -658,10 +614,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>模组光效</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>green</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -685,6 +637,54 @@
   </si>
   <si>
     <t>2022.06.16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Potential</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Star</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modules</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modules Stage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modules Shining</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Illustration</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1119,15 +1119,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2">
         <v>1618440</v>
@@ -1135,39 +1135,39 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B7" s="2">
         <v>170</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2">
         <v>170</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2">
         <v>150</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B10" s="2">
         <v>60</v>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B11" s="2">
         <v>25</v>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B12" s="2">
         <v>147</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2">
         <v>69</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B14" s="2">
         <v>150</v>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2">
         <v>400</v>
@@ -1249,8 +1249,8 @@
   <dimension ref="A1:L115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1262,33 +1262,33 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="5"/>
       <c r="E1" s="7"/>
       <c r="F1" s="15" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
       <c r="I1" s="10" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="K1" s="9"/>
       <c r="L1" s="11" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B2" s="6">
         <v>6</v>
@@ -1312,57 +1312,57 @@
         <v>10</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J2" s="6">
         <v>1</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="12" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>59</v>
+        <v>178</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>180</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>179</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>0</v>
+        <v>182</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>4</v>
+        <v>184</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>5</v>
+        <v>185</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>189</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>49</v>
+        <v>186</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>76</v>
+        <v>187</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -1386,12 +1386,12 @@
         <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -1415,21 +1415,21 @@
         <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J5" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="K5">
         <v>3</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -1453,12 +1453,12 @@
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1482,12 +1482,12 @@
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1511,12 +1511,12 @@
         <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -1540,21 +1540,21 @@
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J9" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -1578,21 +1578,21 @@
         <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J10" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="K10">
         <v>1</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -1616,12 +1616,12 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -1645,12 +1645,12 @@
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1674,12 +1674,12 @@
         <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -1703,21 +1703,21 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J14" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="K14">
         <v>2</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>6</v>
@@ -1741,12 +1741,12 @@
         <v>10</v>
       </c>
       <c r="I15" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -1770,12 +1770,12 @@
         <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -1799,21 +1799,21 @@
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J17" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="K17">
         <v>3</v>
       </c>
       <c r="L17" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>6</v>
@@ -1837,21 +1837,21 @@
         <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J18" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="K18">
         <v>1</v>
       </c>
       <c r="L18" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B19">
         <v>6</v>
@@ -1875,12 +1875,12 @@
         <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -1904,12 +1904,12 @@
         <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1933,12 +1933,12 @@
         <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -1962,12 +1962,12 @@
         <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B23">
         <v>6</v>
@@ -1991,21 +1991,21 @@
         <v>10</v>
       </c>
       <c r="I23" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J23" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="K23">
         <v>1</v>
       </c>
       <c r="L23" s="14" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -2029,21 +2029,21 @@
         <v>10</v>
       </c>
       <c r="I24" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J24" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="K24">
         <v>1</v>
       </c>
       <c r="L24" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B25">
         <v>6</v>
@@ -2067,21 +2067,21 @@
         <v>10</v>
       </c>
       <c r="I25" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J25" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="K25">
         <v>1</v>
       </c>
       <c r="L25" s="14" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B26">
         <v>6</v>
@@ -2105,12 +2105,12 @@
         <v>10</v>
       </c>
       <c r="I26" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>6</v>
@@ -2134,21 +2134,21 @@
         <v>10</v>
       </c>
       <c r="I27" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J27" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="K27">
         <v>1</v>
       </c>
       <c r="L27" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -2172,21 +2172,21 @@
         <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J28" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="K28">
         <v>1</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B29">
         <v>6</v>
@@ -2210,21 +2210,21 @@
         <v>10</v>
       </c>
       <c r="I29" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="J29" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="K29">
         <v>1</v>
       </c>
       <c r="L29" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B30">
         <v>6</v>
@@ -2248,12 +2248,12 @@
         <v>10</v>
       </c>
       <c r="I30" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B31">
         <v>6</v>
@@ -2277,12 +2277,12 @@
         <v>10</v>
       </c>
       <c r="I31" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B32">
         <v>6</v>
@@ -2306,12 +2306,12 @@
         <v>10</v>
       </c>
       <c r="I32" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B33">
         <v>6</v>
@@ -2335,12 +2335,12 @@
         <v>10</v>
       </c>
       <c r="I33" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B34">
         <v>6</v>
@@ -2364,12 +2364,12 @@
         <v>10</v>
       </c>
       <c r="I34" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B35">
         <v>6</v>
@@ -2393,21 +2393,21 @@
         <v>10</v>
       </c>
       <c r="I35" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J35" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="K35">
         <v>1</v>
       </c>
       <c r="L35" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B36">
         <v>6</v>
@@ -2431,12 +2431,12 @@
         <v>10</v>
       </c>
       <c r="I36" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B37">
         <v>6</v>
@@ -2460,12 +2460,12 @@
         <v>10</v>
       </c>
       <c r="I37" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B38">
         <v>6</v>
@@ -2489,12 +2489,12 @@
         <v>10</v>
       </c>
       <c r="I38" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B39">
         <v>6</v>
@@ -2518,21 +2518,21 @@
         <v>10</v>
       </c>
       <c r="I39" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J39" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="K39">
         <v>1</v>
       </c>
       <c r="L39" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B40">
         <v>6</v>
@@ -2556,12 +2556,12 @@
         <v>10</v>
       </c>
       <c r="I40" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B41">
         <v>6</v>
@@ -2585,12 +2585,12 @@
         <v>10</v>
       </c>
       <c r="I41" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B42">
         <v>6</v>
@@ -2614,21 +2614,21 @@
         <v>10</v>
       </c>
       <c r="I42" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J42" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="K42">
         <v>1</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B43">
         <v>6</v>
@@ -2652,21 +2652,21 @@
         <v>10</v>
       </c>
       <c r="I43" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J43" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="K43">
         <v>1</v>
       </c>
       <c r="L43" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B44">
         <v>6</v>
@@ -2690,12 +2690,12 @@
         <v>10</v>
       </c>
       <c r="I44" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B45">
         <v>6</v>
@@ -2719,21 +2719,21 @@
         <v>10</v>
       </c>
       <c r="I45" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J45" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="K45">
         <v>1</v>
       </c>
       <c r="L45" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B46">
         <v>6</v>
@@ -2757,12 +2757,12 @@
         <v>10</v>
       </c>
       <c r="I46" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B47">
         <v>6</v>
@@ -2786,21 +2786,21 @@
         <v>10</v>
       </c>
       <c r="I47" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J47" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="K47">
         <v>1</v>
       </c>
       <c r="L47" s="14" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B48">
         <v>6</v>
@@ -2824,12 +2824,12 @@
         <v>10</v>
       </c>
       <c r="I48" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B49">
         <v>6</v>
@@ -2853,21 +2853,21 @@
         <v>10</v>
       </c>
       <c r="I49" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J49" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="K49">
         <v>1</v>
       </c>
       <c r="L49" s="14" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B50">
         <v>6</v>
@@ -2891,21 +2891,21 @@
         <v>10</v>
       </c>
       <c r="I50" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="J50" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="K50">
         <v>1</v>
       </c>
       <c r="L50" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B51">
         <v>6</v>
@@ -2929,12 +2929,12 @@
         <v>10</v>
       </c>
       <c r="I51" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B52">
         <v>6</v>
@@ -2958,21 +2958,21 @@
         <v>10</v>
       </c>
       <c r="I52" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J52" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="K52">
         <v>1</v>
       </c>
       <c r="L52" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B53">
         <v>6</v>
@@ -2996,21 +2996,21 @@
         <v>10</v>
       </c>
       <c r="I53" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J53" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="K53">
         <v>3</v>
       </c>
       <c r="L53" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B54">
         <v>6</v>
@@ -3034,21 +3034,21 @@
         <v>10</v>
       </c>
       <c r="I54" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J54" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="K54">
         <v>1</v>
       </c>
       <c r="L54" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B55">
         <v>6</v>
@@ -3072,12 +3072,12 @@
         <v>10</v>
       </c>
       <c r="I55" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B56">
         <v>6</v>
@@ -3101,12 +3101,12 @@
         <v>10</v>
       </c>
       <c r="I56" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B57">
         <v>6</v>
@@ -3130,12 +3130,12 @@
         <v>10</v>
       </c>
       <c r="I57" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B58">
         <v>6</v>
@@ -3159,21 +3159,21 @@
         <v>10</v>
       </c>
       <c r="I58" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J58" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="K58">
         <v>1</v>
       </c>
       <c r="L58" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B59">
         <v>6</v>
@@ -3197,21 +3197,21 @@
         <v>10</v>
       </c>
       <c r="I59" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="J59" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="K59">
         <v>1</v>
       </c>
       <c r="L59" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B60">
         <v>6</v>
@@ -3235,21 +3235,21 @@
         <v>10</v>
       </c>
       <c r="I60" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J60" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="K60">
         <v>1</v>
       </c>
       <c r="L60" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B61">
         <v>6</v>
@@ -3273,12 +3273,12 @@
         <v>10</v>
       </c>
       <c r="I61" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B62">
         <v>6</v>
@@ -3302,12 +3302,12 @@
         <v>10</v>
       </c>
       <c r="I62" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B63">
         <v>5</v>
@@ -3331,12 +3331,12 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B64">
         <v>5</v>
@@ -3360,12 +3360,12 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B65">
         <v>5</v>
@@ -3389,12 +3389,12 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B66">
         <v>5</v>
@@ -3418,12 +3418,12 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B67">
         <v>5</v>
@@ -3447,12 +3447,12 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B68">
         <v>5</v>
@@ -3476,21 +3476,21 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J68" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="K68">
         <v>1</v>
       </c>
       <c r="L68" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B69">
         <v>5</v>
@@ -3514,12 +3514,12 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B70">
         <v>5</v>
@@ -3543,12 +3543,12 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B71">
         <v>5</v>
@@ -3572,12 +3572,12 @@
         <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B72">
         <v>5</v>
@@ -3601,12 +3601,12 @@
         <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B73">
         <v>5</v>
@@ -3630,21 +3630,21 @@
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J73" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="K73">
         <v>1</v>
       </c>
       <c r="L73" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B74">
         <v>5</v>
@@ -3668,12 +3668,12 @@
         <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B75">
         <v>5</v>
@@ -3697,21 +3697,21 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J75" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="K75">
         <v>3</v>
       </c>
       <c r="L75" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B76">
         <v>5</v>
@@ -3735,12 +3735,12 @@
         <v>0</v>
       </c>
       <c r="I76" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B77">
         <v>5</v>
@@ -3764,12 +3764,12 @@
         <v>0</v>
       </c>
       <c r="I77" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B78">
         <v>5</v>
@@ -3793,21 +3793,21 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="J78" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="K78">
         <v>1</v>
       </c>
       <c r="L78" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B79">
         <v>5</v>
@@ -3831,12 +3831,12 @@
         <v>0</v>
       </c>
       <c r="I79" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B80">
         <v>5</v>
@@ -3860,21 +3860,21 @@
         <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J80" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="K80">
         <v>1</v>
       </c>
       <c r="L80" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B81">
         <v>5</v>
@@ -3898,12 +3898,12 @@
         <v>0</v>
       </c>
       <c r="I81" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B82">
         <v>5</v>
@@ -3927,12 +3927,12 @@
         <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B83">
         <v>5</v>
@@ -3956,21 +3956,21 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J83" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="K83">
         <v>1</v>
       </c>
       <c r="L83" s="14" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B84">
         <v>5</v>
@@ -3994,12 +3994,12 @@
         <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B85">
         <v>5</v>
@@ -4023,12 +4023,12 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B86">
         <v>5</v>
@@ -4052,12 +4052,12 @@
         <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B87">
         <v>5</v>
@@ -4081,12 +4081,12 @@
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B88">
         <v>5</v>
@@ -4110,12 +4110,12 @@
         <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B89">
         <v>5</v>
@@ -4139,12 +4139,12 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B90">
         <v>5</v>
@@ -4168,21 +4168,21 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J90" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="K90">
         <v>1</v>
       </c>
       <c r="L90" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B91">
         <v>5</v>
@@ -4206,12 +4206,12 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B92">
         <v>5</v>
@@ -4235,21 +4235,21 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J92" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="K92">
         <v>1</v>
       </c>
       <c r="L92" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B93">
         <v>5</v>
@@ -4273,12 +4273,12 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B94">
         <v>5</v>
@@ -4302,21 +4302,21 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J94" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="K94">
         <v>1</v>
       </c>
       <c r="L94" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B95">
         <v>5</v>
@@ -4340,21 +4340,21 @@
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J95" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="K95">
         <v>1</v>
       </c>
       <c r="L95" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B96">
         <v>5</v>
@@ -4378,21 +4378,21 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J96" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="K96">
         <v>1</v>
       </c>
       <c r="L96" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B97">
         <v>5</v>
@@ -4416,21 +4416,21 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J97" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="K97">
         <v>1</v>
       </c>
       <c r="L97" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B98">
         <v>5</v>
@@ -4454,12 +4454,12 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B99">
         <v>5</v>
@@ -4483,12 +4483,12 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B100">
         <v>5</v>
@@ -4512,12 +4512,12 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B101">
         <v>4</v>
@@ -4541,12 +4541,12 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B102">
         <v>4</v>
@@ -4570,12 +4570,12 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B103">
         <v>4</v>
@@ -4599,21 +4599,21 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J103" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="K103">
         <v>1</v>
       </c>
       <c r="L103" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B104">
         <v>4</v>
@@ -4637,12 +4637,12 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B105">
         <v>4</v>
@@ -4666,12 +4666,12 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B106">
         <v>4</v>
@@ -4695,12 +4695,12 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B107">
         <v>4</v>
@@ -4724,12 +4724,12 @@
         <v>0</v>
       </c>
       <c r="I107" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B108">
         <v>4</v>
@@ -4753,21 +4753,21 @@
         <v>0</v>
       </c>
       <c r="I108" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J108" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="K108">
         <v>1</v>
       </c>
       <c r="L108" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B109">
         <v>4</v>
@@ -4791,21 +4791,21 @@
         <v>0</v>
       </c>
       <c r="I109" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="J109" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="K109">
         <v>1</v>
       </c>
       <c r="L109" s="14" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B110">
         <v>4</v>
@@ -4829,12 +4829,12 @@
         <v>0</v>
       </c>
       <c r="I110" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B111">
         <v>4</v>
@@ -4858,21 +4858,21 @@
         <v>0</v>
       </c>
       <c r="I111" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="J111" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="K111">
         <v>1</v>
       </c>
       <c r="L111" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B112">
         <v>4</v>
@@ -4896,21 +4896,21 @@
         <v>0</v>
       </c>
       <c r="I112" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J112" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="K112">
         <v>1</v>
       </c>
       <c r="L112" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B113">
         <v>4</v>
@@ -4934,21 +4934,21 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J113" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="K113">
         <v>1</v>
       </c>
       <c r="L113" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B114">
         <v>4</v>
@@ -4972,21 +4972,21 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J114" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="K114">
         <v>1</v>
       </c>
       <c r="L114" s="14" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B115">
         <v>4</v>
@@ -5010,7 +5010,7 @@
         <v>0</v>
       </c>
       <c r="I115" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -5024,7 +5024,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 I4:I115" xr:uid="{A8166145-CD83-4526-BE5E-2B372ACB9134}">
       <formula1>"elite1,elite2,skin1,skin2,skin3"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K2 B101:G115 J101:K115 J118:K1048576 B118:H1048576 J1:J3 B1:H3" xr:uid="{067929F4-68AD-4FCF-9645-B8AA87BCECB2}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K2 B101:G115 J101:K115 J118:K1048576 B118:H1048576 E1:H2 B1:B2 C1:C2 D1:D2 J1:J2" xr:uid="{067929F4-68AD-4FCF-9645-B8AA87BCECB2}">
       <formula1>0</formula1>
       <formula2>90</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Profile picture newly added
</commit_message>
<xml_diff>
--- a/Source/arkD.xlsx
+++ b/Source/arkD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37b141e1e60375e0/Arknights/ArknightsIDcard-Ebranch/ArknightsIDCard/Source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="13_ncr:1_{315788DD-20D3-4743-AE64-E916F6B19C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F67A4D5-1A13-4300-B98F-37F640365348}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{315788DD-20D3-4743-AE64-E916F6B19C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BCAF7B8-75B4-4DE8-92AB-0A0597D22A8A}"/>
   <bookViews>
-    <workbookView xWindow="-16370" yWindow="7930" windowWidth="14840" windowHeight="10080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="11596" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="其他信息" sheetId="2" r:id="rId1"/>
@@ -1435,8 +1435,8 @@
   <dimension ref="A1:L140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I108" sqref="I108"/>
+      <pane ySplit="3" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -5986,7 +5986,7 @@
         <v>70</v>
       </c>
       <c r="F139">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G139">
         <v>10</v>

</xml_diff>